<commit_message>
Update MEIC scaling inventory (#246)
* Add newer MEIC inventory
* Adjust mappings to be more consistent between two MEIC versions
</commit_message>
<xml_diff>
--- a/input/emissions-inventories/China/CEDS_MEIC_Emissions_2rdLevel_20160226_plus.xlsx
+++ b/input/emissions-inventories/China/CEDS_MEIC_Emissions_2rdLevel_20160226_plus.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Documents/Information &amp; Documents/CEDS_Project/CEDS/input/emissions-inventories/China/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D327E81-107E-BD4C-AF58-6BEC0A3743BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SourceMapping" sheetId="1" r:id="rId1"/>
@@ -15,8 +21,16 @@
   <externalReferences>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -635,7 +649,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1016,27 +1030,35 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="U.SO2_Metal_Smelting.csv"/>
+      <sheetName val="U.SO2_Metal_Smelting"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="20">
+          <cell r="E20">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="25">
           <cell r="FG25">
-            <v>3587.9069420000001</v>
+            <v>3239.0086200000001</v>
           </cell>
           <cell r="FI25">
-            <v>4351.7106649999996</v>
+            <v>2934.0094600000002</v>
           </cell>
           <cell r="FK25">
-            <v>4429.6757349999998</v>
+            <v>2530.7018499999999</v>
           </cell>
         </row>
       </sheetData>
@@ -1300,21 +1322,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.6640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="49.5" style="2" customWidth="1"/>
@@ -1322,7 +1344,7 @@
     <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>62</v>
       </c>
@@ -1333,7 +1355,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>64</v>
       </c>
@@ -1347,7 +1369,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>66</v>
       </c>
@@ -1361,7 +1383,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>68</v>
       </c>
@@ -1375,13 +1397,13 @@
       <c r="F4" s="10"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="22"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>70</v>
       </c>
@@ -1389,7 +1411,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1397,31 +1419,31 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="18"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="18"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="18"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>154</v>
       </c>
@@ -1429,37 +1451,37 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="18"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="18"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="18"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="18"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="18"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>14</v>
       </c>
@@ -1467,19 +1489,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="22"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="22"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>74</v>
       </c>
@@ -1487,7 +1509,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>76</v>
       </c>
@@ -1495,13 +1517,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="22"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>161</v>
       </c>
@@ -1509,7 +1531,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>79</v>
       </c>
@@ -1517,7 +1539,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>155</v>
       </c>
@@ -1525,7 +1547,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>21</v>
       </c>
@@ -1533,7 +1555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>82</v>
       </c>
@@ -1541,19 +1563,19 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="22"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="22"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>85</v>
       </c>
@@ -1561,7 +1583,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>25</v>
       </c>
@@ -1569,7 +1591,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>87</v>
       </c>
@@ -1577,7 +1599,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>89</v>
       </c>
@@ -1585,19 +1607,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="22"/>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="22"/>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>30</v>
       </c>
@@ -1605,7 +1627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>32</v>
       </c>
@@ -1613,7 +1635,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>33</v>
       </c>
@@ -1621,7 +1643,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>34</v>
       </c>
@@ -1629,7 +1651,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>35</v>
       </c>
@@ -1637,7 +1659,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>36</v>
       </c>
@@ -1645,7 +1667,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
@@ -1653,7 +1675,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>38</v>
       </c>
@@ -1661,7 +1683,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="45">
+    <row r="45" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>98</v>
       </c>
@@ -1669,7 +1691,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>100</v>
       </c>
@@ -1677,7 +1699,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>102</v>
       </c>
@@ -1685,7 +1707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>39</v>
       </c>
@@ -1693,13 +1715,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B49" s="22"/>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -1707,7 +1729,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>42</v>
       </c>
@@ -1715,13 +1737,13 @@
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="22"/>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>44</v>
       </c>
@@ -1729,19 +1751,19 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B54" s="22"/>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B55" s="22"/>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>46</v>
       </c>
@@ -1749,13 +1771,13 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B57" s="22"/>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>48</v>
       </c>
@@ -1763,25 +1785,25 @@
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B59" s="22"/>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>111</v>
       </c>
       <c r="B60" s="22"/>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B61" s="22"/>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>51</v>
       </c>
@@ -1800,21 +1822,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.6640625" style="12" customWidth="1"/>
     <col min="2" max="8" width="19.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>113</v>
       </c>
@@ -1840,7 +1862,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>156</v>
       </c>
@@ -1866,7 +1888,7 @@
         <v>52.124854415422305</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1892,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
@@ -1918,7 +1940,7 @@
         <v>17.79707568102458</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
@@ -1944,7 +1966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>70</v>
       </c>
@@ -1970,7 +1992,7 @@
         <v>242148.31293439865</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1996,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -2022,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -2048,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -2074,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>116</v>
       </c>
@@ -2100,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>72</v>
       </c>
@@ -2126,7 +2148,7 @@
         <v>12485.91032409668</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
@@ -2152,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
@@ -2178,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -2204,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -2230,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -2256,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>14</v>
       </c>
@@ -2282,7 +2304,7 @@
         <v>67881.693745168857</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -2308,7 +2330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
@@ -2334,7 +2356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>74</v>
       </c>
@@ -2360,7 +2382,7 @@
         <v>72818.305900519976</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>76</v>
       </c>
@@ -2386,7 +2408,7 @@
         <v>2508.6471470594406</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
@@ -2412,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>161</v>
       </c>
@@ -2438,7 +2460,7 @@
         <v>1015.086017306134</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>20</v>
       </c>
@@ -2464,7 +2486,7 @@
         <v>23292.268866300583</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>119</v>
       </c>
@@ -2490,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>21</v>
       </c>
@@ -2516,7 +2538,7 @@
         <v>2513788.2144603585</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>82</v>
       </c>
@@ -2542,7 +2564,7 @@
         <v>6006.1227464675903</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>23</v>
       </c>
@@ -2568,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>24</v>
       </c>
@@ -2594,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>85</v>
       </c>
@@ -2620,7 +2642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>124</v>
       </c>
@@ -2646,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>27</v>
       </c>
@@ -2672,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>89</v>
       </c>
@@ -2698,7 +2720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>28</v>
       </c>
@@ -2724,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>29</v>
       </c>
@@ -2750,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>30</v>
       </c>
@@ -2776,7 +2798,7 @@
         <v>22402.999715030193</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>128</v>
       </c>
@@ -2802,7 +2824,7 @@
         <v>1935.8960747718811</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>33</v>
       </c>
@@ -2828,7 +2850,7 @@
         <v>174773.02461004257</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>34</v>
       </c>
@@ -2854,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>35</v>
       </c>
@@ -2880,7 +2902,7 @@
         <v>51753.531762309372</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>36</v>
       </c>
@@ -2906,13 +2928,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="34">
-        <f>[1]U.SO2_Metal_Smelting.csv!$FG$25*1000-B41</f>
-        <v>2800612.997282593</v>
+        <f>[1]U.SO2_Metal_Smelting!$FG$25*1000-B41</f>
+        <v>2451714.6752825929</v>
       </c>
       <c r="C43" s="34">
         <v>0</v>
@@ -2933,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>38</v>
       </c>
@@ -2959,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>98</v>
       </c>
@@ -2985,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>100</v>
       </c>
@@ -3011,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>102</v>
       </c>
@@ -3037,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>39</v>
       </c>
@@ -3063,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>40</v>
       </c>
@@ -3089,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -3115,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>42</v>
       </c>
@@ -3141,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>43</v>
       </c>
@@ -3167,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>44</v>
       </c>
@@ -3193,7 +3215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>108</v>
       </c>
@@ -3219,7 +3241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>45</v>
       </c>
@@ -3245,7 +3267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>46</v>
       </c>
@@ -3271,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>47</v>
       </c>
@@ -3297,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>48</v>
       </c>
@@ -3323,7 +3345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>49</v>
       </c>
@@ -3349,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>111</v>
       </c>
@@ -3375,7 +3397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>50</v>
       </c>
@@ -3401,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>51</v>
       </c>
@@ -3427,10 +3449,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" s="1" customFormat="1">
+    <row r="65" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <f>SUM(B2:B62)/1000</f>
-        <v>34187.837636961442</v>
+        <v>33838.939314961448</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" ref="C65:H65" si="0">SUM(C2:C62)/1000</f>
@@ -3469,21 +3491,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView topLeftCell="A27" zoomScale="101" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.6640625" style="12" customWidth="1"/>
     <col min="2" max="8" width="19.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>113</v>
       </c>
@@ -3509,7 +3531,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
@@ -3535,7 +3557,7 @@
         <v>17.373511559329927</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -3561,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>2</v>
       </c>
@@ -3587,7 +3609,7 @@
         <v>25.502136757497283</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
@@ -3613,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>115</v>
       </c>
@@ -3639,7 +3661,7 @@
         <v>251984.54051589966</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -3665,7 +3687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -3691,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -3717,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -3743,7 +3765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>116</v>
       </c>
@@ -3769,7 +3791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>117</v>
       </c>
@@ -3795,7 +3817,7 @@
         <v>13905.176273584366</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
@@ -3821,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
@@ -3847,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -3873,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -3899,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -3925,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>14</v>
       </c>
@@ -3951,7 +3973,7 @@
         <v>70982.890945868596</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -3977,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
@@ -4003,7 +4025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>17</v>
       </c>
@@ -4029,7 +4051,7 @@
         <v>52990.77123650947</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>18</v>
       </c>
@@ -4055,7 +4077,7 @@
         <v>2437.7317457199097</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
@@ -4081,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>161</v>
       </c>
@@ -4107,7 +4129,7 @@
         <v>1285.9695615013015</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>118</v>
       </c>
@@ -4133,7 +4155,7 @@
         <v>22171.741340637207</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>119</v>
       </c>
@@ -4159,7 +4181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>120</v>
       </c>
@@ -4185,7 +4207,7 @@
         <v>2481488.5505911168</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>121</v>
       </c>
@@ -4211,7 +4233,7 @@
         <v>6814.0273003578186</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>23</v>
       </c>
@@ -4237,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>122</v>
       </c>
@@ -4263,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>123</v>
       </c>
@@ -4289,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>124</v>
       </c>
@@ -4315,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>125</v>
       </c>
@@ -4341,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>126</v>
       </c>
@@ -4367,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>28</v>
       </c>
@@ -4393,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>29</v>
       </c>
@@ -4419,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>127</v>
       </c>
@@ -4445,7 +4467,7 @@
         <v>13415.443477615714</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>128</v>
       </c>
@@ -4471,7 +4493,7 @@
         <v>2034.1060981750488</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>129</v>
       </c>
@@ -4497,7 +4519,7 @@
         <v>177882.07409954071</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>34</v>
       </c>
@@ -4523,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>35</v>
       </c>
@@ -4549,7 +4571,7 @@
         <v>62321.848316989839</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>36</v>
       </c>
@@ -4575,13 +4597,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="34">
-        <f>[1]U.SO2_Metal_Smelting.csv!$FI$25*1000-B41</f>
-        <v>3446305.6850805664</v>
+        <f>[1]U.SO2_Metal_Smelting!$FI$25*1000-B41</f>
+        <v>2028604.4800805668</v>
       </c>
       <c r="C43" s="34">
         <v>0</v>
@@ -4602,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>38</v>
       </c>
@@ -4628,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>130</v>
       </c>
@@ -4654,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>100</v>
       </c>
@@ -4680,7 +4702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>131</v>
       </c>
@@ -4706,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>39</v>
       </c>
@@ -4732,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>40</v>
       </c>
@@ -4758,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -4784,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>42</v>
       </c>
@@ -4810,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>43</v>
       </c>
@@ -4836,7 +4858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>44</v>
       </c>
@@ -4862,7 +4884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>132</v>
       </c>
@@ -4888,7 +4910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>45</v>
       </c>
@@ -4914,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>46</v>
       </c>
@@ -4940,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>47</v>
       </c>
@@ -4966,7 +4988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>48</v>
       </c>
@@ -4992,7 +5014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>49</v>
       </c>
@@ -5018,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>133</v>
       </c>
@@ -5044,7 +5066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>50</v>
       </c>
@@ -5070,7 +5092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>51</v>
       </c>
@@ -5096,10 +5118,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" s="1" customFormat="1">
+    <row r="65" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <f>SUM(B2:B62)/1000</f>
-        <v>31911.697557558429</v>
+        <v>30493.996352558432</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" ref="C65:H65" si="0">SUM(C2:C62)/1000</f>
@@ -5139,21 +5161,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.6640625" style="12" customWidth="1"/>
     <col min="2" max="8" width="19.1640625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>134</v>
       </c>
@@ -5179,7 +5201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>135</v>
       </c>
@@ -5205,7 +5227,7 @@
         <v>6.8272470724768937</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>136</v>
       </c>
@@ -5231,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>137</v>
       </c>
@@ -5257,7 +5279,7 @@
         <v>23.344314957794268</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
@@ -5283,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>158</v>
       </c>
@@ -5309,7 +5331,7 @@
         <v>274237.90397644043</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -5335,7 +5357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -5361,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -5387,7 +5409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
@@ -5413,7 +5435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>157</v>
       </c>
@@ -5439,7 +5461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>72</v>
       </c>
@@ -5465,7 +5487,7 @@
         <v>16615.301568031311</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
@@ -5491,7 +5513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
@@ -5517,7 +5539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -5543,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -5569,7 +5591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -5595,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
         <v>14</v>
       </c>
@@ -5621,7 +5643,7 @@
         <v>79291.143737397157</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
@@ -5647,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>16</v>
       </c>
@@ -5673,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="19" t="s">
         <v>138</v>
       </c>
@@ -5699,7 +5721,7 @@
         <v>44585.984474747253</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="19" t="s">
         <v>139</v>
       </c>
@@ -5725,7 +5747,7 @@
         <v>2300.3896576166153</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
         <v>19</v>
       </c>
@@ -5751,7 +5773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="19" t="s">
         <v>161</v>
       </c>
@@ -5777,7 +5799,7 @@
         <v>1665.4569050705959</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="19" t="s">
         <v>140</v>
       </c>
@@ -5803,7 +5825,7 @@
         <v>22041.620704889297</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>141</v>
       </c>
@@ -5829,7 +5851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
         <v>142</v>
       </c>
@@ -5855,7 +5877,7 @@
         <v>2465075.5727499053</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>82</v>
       </c>
@@ -5881,7 +5903,7 @@
         <v>7691.4222388267517</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>23</v>
       </c>
@@ -5907,7 +5929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>143</v>
       </c>
@@ -5933,7 +5955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>144</v>
       </c>
@@ -5959,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
         <v>145</v>
       </c>
@@ -5985,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
         <v>146</v>
       </c>
@@ -6011,7 +6033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
         <v>147</v>
       </c>
@@ -6037,7 +6059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>28</v>
       </c>
@@ -6063,7 +6085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>29</v>
       </c>
@@ -6089,7 +6111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
         <v>148</v>
       </c>
@@ -6115,7 +6137,7 @@
         <v>12987.964296636721</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
         <v>149</v>
       </c>
@@ -6141,7 +6163,7 @@
         <v>2214.1579561233521</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>150</v>
       </c>
@@ -6167,7 +6189,7 @@
         <v>180991.11910295486</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
         <v>34</v>
       </c>
@@ -6193,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
         <v>35</v>
       </c>
@@ -6219,11 +6241,12 @@
         <v>68139.499520309269</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="34">
+        <f>[1]U.SO2_Metal_Smelting!$E$20</f>
         <v>0</v>
       </c>
       <c r="C42" s="34">
@@ -6245,13 +6268,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="34">
-        <f>[1]U.SO2_Metal_Smelting.csv!$FK$25*1000-B41</f>
-        <v>3726681.5222924799</v>
+        <f>[1]U.SO2_Metal_Smelting!$FK$25*1000-B41</f>
+        <v>1827707.6372924806</v>
       </c>
       <c r="C43" s="34">
         <v>0</v>
@@ -6272,7 +6295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
         <v>38</v>
       </c>
@@ -6298,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>98</v>
       </c>
@@ -6324,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
         <v>114</v>
       </c>
@@ -6350,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
         <v>151</v>
       </c>
@@ -6376,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
         <v>39</v>
       </c>
@@ -6402,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>40</v>
       </c>
@@ -6428,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
         <v>41</v>
       </c>
@@ -6454,7 +6477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>42</v>
       </c>
@@ -6480,7 +6503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
         <v>43</v>
       </c>
@@ -6506,7 +6529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="17" t="s">
         <v>44</v>
       </c>
@@ -6532,7 +6555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
         <v>152</v>
       </c>
@@ -6558,7 +6581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="21" t="s">
         <v>45</v>
       </c>
@@ -6584,7 +6607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="23" t="s">
         <v>46</v>
       </c>
@@ -6610,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
         <v>47</v>
       </c>
@@ -6636,7 +6659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>48</v>
       </c>
@@ -6662,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="21" t="s">
         <v>49</v>
       </c>
@@ -6688,7 +6711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
         <v>153</v>
       </c>
@@ -6714,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>50</v>
       </c>
@@ -6740,7 +6763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="27" t="s">
         <v>51</v>
       </c>
@@ -6766,10 +6789,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <f>SUM(B2:B62)/1000</f>
-        <v>33410.959534006986</v>
+        <v>31511.985649006991</v>
       </c>
       <c r="C65" s="1">
         <f t="shared" ref="C65:H65" si="0">SUM(C2:C62)/1000</f>

</xml_diff>